<commit_message>
update auffrischen kreisebene and kv
</commit_message>
<xml_diff>
--- a/data/auffrischen_kw_bl.xlsx
+++ b/data/auffrischen_kw_bl.xlsx
@@ -506,49 +506,49 @@
         <v>994296</v>
       </c>
       <c r="C2" t="n">
-        <v>384135</v>
+        <v>458045</v>
       </c>
       <c r="D2" t="n">
-        <v>610161</v>
+        <v>536251</v>
       </c>
       <c r="E2" t="n">
-        <v>0.613661324193198</v>
+        <v>0.539327323050681</v>
       </c>
       <c r="F2" t="n">
-        <v>191315</v>
+        <v>185156</v>
       </c>
       <c r="G2" t="n">
-        <v>296892</v>
+        <v>290733</v>
       </c>
       <c r="H2" t="n">
-        <v>329996</v>
+        <v>323837</v>
       </c>
       <c r="I2" t="n">
-        <v>468555</v>
+        <v>462396</v>
       </c>
       <c r="J2" t="n">
-        <v>415893</v>
+        <v>409734</v>
       </c>
       <c r="K2" t="n">
-        <v>615083</v>
+        <v>608924</v>
       </c>
       <c r="L2" t="n">
-        <v>564424</v>
+        <v>558265</v>
       </c>
       <c r="M2" t="n">
-        <v>517538</v>
+        <v>511379</v>
       </c>
       <c r="N2" t="n">
-        <v>453026</v>
+        <v>446867</v>
       </c>
       <c r="O2" t="n">
-        <v>474309</v>
+        <v>468150</v>
       </c>
       <c r="P2" t="n">
-        <v>521989</v>
+        <v>515830</v>
       </c>
       <c r="Q2" t="n">
-        <v>436967</v>
+        <v>430808</v>
       </c>
     </row>
     <row r="3">
@@ -559,49 +559,49 @@
         <v>1175360</v>
       </c>
       <c r="C3" t="n">
-        <v>484787</v>
+        <v>591451</v>
       </c>
       <c r="D3" t="n">
-        <v>690573</v>
+        <v>583909</v>
       </c>
       <c r="E3" t="n">
-        <v>0.587541689354751</v>
+        <v>0.496791621290498</v>
       </c>
       <c r="F3" t="n">
-        <v>251398</v>
+        <v>242509</v>
       </c>
       <c r="G3" t="n">
-        <v>260009</v>
+        <v>251120</v>
       </c>
       <c r="H3" t="n">
-        <v>399183</v>
+        <v>390294</v>
       </c>
       <c r="I3" t="n">
-        <v>622516</v>
+        <v>613627</v>
       </c>
       <c r="J3" t="n">
-        <v>580908</v>
+        <v>572019</v>
       </c>
       <c r="K3" t="n">
-        <v>669890</v>
+        <v>661001</v>
       </c>
       <c r="L3" t="n">
-        <v>660809</v>
+        <v>651920</v>
       </c>
       <c r="M3" t="n">
-        <v>653471</v>
+        <v>644582</v>
       </c>
       <c r="N3" t="n">
-        <v>446439</v>
+        <v>437550</v>
       </c>
       <c r="O3" t="n">
-        <v>468403</v>
+        <v>459514</v>
       </c>
       <c r="P3" t="n">
-        <v>432393</v>
+        <v>423504</v>
       </c>
       <c r="Q3" t="n">
-        <v>426527</v>
+        <v>417638</v>
       </c>
     </row>
     <row r="4">
@@ -612,49 +612,49 @@
         <v>406949</v>
       </c>
       <c r="C4" t="n">
-        <v>232779</v>
+        <v>259157</v>
       </c>
       <c r="D4" t="n">
-        <v>174170</v>
+        <v>147792</v>
       </c>
       <c r="E4" t="n">
-        <v>0.427989748101113</v>
+        <v>0.363170815016132</v>
       </c>
       <c r="F4" t="n">
-        <v>65556</v>
+        <v>63358</v>
       </c>
       <c r="G4" t="n">
-        <v>71838</v>
+        <v>69640</v>
       </c>
       <c r="H4" t="n">
-        <v>96420</v>
+        <v>94222</v>
       </c>
       <c r="I4" t="n">
-        <v>115343</v>
+        <v>113145</v>
       </c>
       <c r="J4" t="n">
-        <v>129040</v>
+        <v>126842</v>
       </c>
       <c r="K4" t="n">
-        <v>168305</v>
+        <v>166107</v>
       </c>
       <c r="L4" t="n">
-        <v>181244</v>
+        <v>179046</v>
       </c>
       <c r="M4" t="n">
-        <v>171033</v>
+        <v>168835</v>
       </c>
       <c r="N4" t="n">
-        <v>144608</v>
+        <v>142410</v>
       </c>
       <c r="O4" t="n">
-        <v>164869</v>
+        <v>162671</v>
       </c>
       <c r="P4" t="n">
-        <v>177182</v>
+        <v>174984</v>
       </c>
       <c r="Q4" t="n">
-        <v>120109</v>
+        <v>117911</v>
       </c>
     </row>
     <row r="5">
@@ -665,49 +665,49 @@
         <v>241717</v>
       </c>
       <c r="C5" t="n">
-        <v>72429</v>
+        <v>86518</v>
       </c>
       <c r="D5" t="n">
-        <v>169288</v>
+        <v>155199</v>
       </c>
       <c r="E5" t="n">
-        <v>0.700356201673858</v>
+        <v>0.642069031139721</v>
       </c>
       <c r="F5" t="n">
-        <v>68721</v>
+        <v>67547</v>
       </c>
       <c r="G5" t="n">
-        <v>74149</v>
+        <v>72975</v>
       </c>
       <c r="H5" t="n">
-        <v>77986</v>
+        <v>76812</v>
       </c>
       <c r="I5" t="n">
-        <v>97986</v>
+        <v>96812</v>
       </c>
       <c r="J5" t="n">
-        <v>100440</v>
+        <v>99266</v>
       </c>
       <c r="K5" t="n">
-        <v>102240</v>
+        <v>101066</v>
       </c>
       <c r="L5" t="n">
-        <v>111233</v>
+        <v>110059</v>
       </c>
       <c r="M5" t="n">
-        <v>111155</v>
+        <v>109981</v>
       </c>
       <c r="N5" t="n">
-        <v>81712</v>
+        <v>80538</v>
       </c>
       <c r="O5" t="n">
-        <v>107084</v>
+        <v>105910</v>
       </c>
       <c r="P5" t="n">
-        <v>116290</v>
+        <v>115116</v>
       </c>
       <c r="Q5" t="n">
-        <v>111308</v>
+        <v>110134</v>
       </c>
     </row>
     <row r="6">
@@ -718,49 +718,49 @@
         <v>82700</v>
       </c>
       <c r="C6" t="n">
-        <v>40559</v>
+        <v>46257</v>
       </c>
       <c r="D6" t="n">
-        <v>42141</v>
+        <v>36443</v>
       </c>
       <c r="E6" t="n">
-        <v>0.50956469165659</v>
+        <v>0.440665054413543</v>
       </c>
       <c r="F6" t="n">
-        <v>21075</v>
+        <v>20600</v>
       </c>
       <c r="G6" t="n">
-        <v>20288</v>
+        <v>19813</v>
       </c>
       <c r="H6" t="n">
-        <v>23768</v>
+        <v>23293</v>
       </c>
       <c r="I6" t="n">
-        <v>29778</v>
+        <v>29303</v>
       </c>
       <c r="J6" t="n">
-        <v>24700</v>
+        <v>24225</v>
       </c>
       <c r="K6" t="n">
-        <v>29314</v>
+        <v>28839</v>
       </c>
       <c r="L6" t="n">
-        <v>25363</v>
+        <v>24888</v>
       </c>
       <c r="M6" t="n">
-        <v>30326</v>
+        <v>29851</v>
       </c>
       <c r="N6" t="n">
-        <v>28705</v>
+        <v>28230</v>
       </c>
       <c r="O6" t="n">
-        <v>41949</v>
+        <v>41474</v>
       </c>
       <c r="P6" t="n">
-        <v>50930</v>
+        <v>50455</v>
       </c>
       <c r="Q6" t="n">
-        <v>38432</v>
+        <v>37957</v>
       </c>
     </row>
     <row r="7">
@@ -771,49 +771,49 @@
         <v>7813381</v>
       </c>
       <c r="C7" t="n">
-        <v>3300010</v>
+        <v>3861486</v>
       </c>
       <c r="D7" t="n">
-        <v>4513371</v>
+        <v>3951895</v>
       </c>
       <c r="E7" t="n">
-        <v>0.577646347976631</v>
+        <v>0.505785523578077</v>
       </c>
       <c r="F7" t="n">
-        <v>1533629</v>
+        <v>1486840</v>
       </c>
       <c r="G7" t="n">
-        <v>1894893</v>
+        <v>1848104</v>
       </c>
       <c r="H7" t="n">
-        <v>2387598</v>
+        <v>2340809</v>
       </c>
       <c r="I7" t="n">
-        <v>3647522</v>
+        <v>3600733</v>
       </c>
       <c r="J7" t="n">
-        <v>3506637</v>
+        <v>3459848</v>
       </c>
       <c r="K7" t="n">
-        <v>4442968</v>
+        <v>4396179</v>
       </c>
       <c r="L7" t="n">
-        <v>4395188</v>
+        <v>4348399</v>
       </c>
       <c r="M7" t="n">
-        <v>3947949</v>
+        <v>3901160</v>
       </c>
       <c r="N7" t="n">
-        <v>3334162</v>
+        <v>3287373</v>
       </c>
       <c r="O7" t="n">
-        <v>3452478</v>
+        <v>3405689</v>
       </c>
       <c r="P7" t="n">
-        <v>3486279</v>
+        <v>3439490</v>
       </c>
       <c r="Q7" t="n">
-        <v>2901881</v>
+        <v>2855092</v>
       </c>
     </row>
     <row r="8">
@@ -824,49 +824,49 @@
         <v>160875</v>
       </c>
       <c r="C8" t="n">
-        <v>72832</v>
+        <v>85379</v>
       </c>
       <c r="D8" t="n">
-        <v>88043</v>
+        <v>75496</v>
       </c>
       <c r="E8" t="n">
-        <v>0.547275835275835</v>
+        <v>0.469283605283605</v>
       </c>
       <c r="F8" t="n">
-        <v>36236</v>
+        <v>35190</v>
       </c>
       <c r="G8" t="n">
-        <v>35586</v>
+        <v>34540</v>
       </c>
       <c r="H8" t="n">
-        <v>60871</v>
+        <v>59825</v>
       </c>
       <c r="I8" t="n">
-        <v>78232</v>
+        <v>77186</v>
       </c>
       <c r="J8" t="n">
-        <v>79989</v>
+        <v>78943</v>
       </c>
       <c r="K8" t="n">
-        <v>88950</v>
+        <v>87904</v>
       </c>
       <c r="L8" t="n">
-        <v>90157</v>
+        <v>89111</v>
       </c>
       <c r="M8" t="n">
-        <v>89136</v>
+        <v>88090</v>
       </c>
       <c r="N8" t="n">
-        <v>59216</v>
+        <v>58170</v>
       </c>
       <c r="O8" t="n">
-        <v>81362</v>
+        <v>80316</v>
       </c>
       <c r="P8" t="n">
-        <v>67416</v>
+        <v>66370</v>
       </c>
       <c r="Q8" t="n">
-        <v>44895</v>
+        <v>43849</v>
       </c>
     </row>
     <row r="9">
@@ -877,49 +877,49 @@
         <v>534750</v>
       </c>
       <c r="C9" t="n">
-        <v>236028</v>
+        <v>273739</v>
       </c>
       <c r="D9" t="n">
-        <v>298722</v>
+        <v>261011</v>
       </c>
       <c r="E9" t="n">
-        <v>0.558619915848527</v>
+        <v>0.488099111734455</v>
       </c>
       <c r="F9" t="n">
-        <v>67398</v>
+        <v>64255</v>
       </c>
       <c r="G9" t="n">
-        <v>129206</v>
+        <v>126063</v>
       </c>
       <c r="H9" t="n">
-        <v>142797</v>
+        <v>139654</v>
       </c>
       <c r="I9" t="n">
-        <v>259674</v>
+        <v>256531</v>
       </c>
       <c r="J9" t="n">
-        <v>213908</v>
+        <v>210765</v>
       </c>
       <c r="K9" t="n">
-        <v>345902</v>
+        <v>342759</v>
       </c>
       <c r="L9" t="n">
-        <v>355467</v>
+        <v>352324</v>
       </c>
       <c r="M9" t="n">
-        <v>307532</v>
+        <v>304389</v>
       </c>
       <c r="N9" t="n">
-        <v>268726</v>
+        <v>265583</v>
       </c>
       <c r="O9" t="n">
-        <v>278942</v>
+        <v>275799</v>
       </c>
       <c r="P9" t="n">
-        <v>286352</v>
+        <v>283209</v>
       </c>
       <c r="Q9" t="n">
-        <v>220592</v>
+        <v>217449</v>
       </c>
     </row>
     <row r="10">
@@ -930,49 +930,49 @@
         <v>138996</v>
       </c>
       <c r="C10" t="n">
-        <v>52923</v>
+        <v>64196</v>
       </c>
       <c r="D10" t="n">
-        <v>86073</v>
+        <v>74800</v>
       </c>
       <c r="E10" t="n">
-        <v>0.619248035914703</v>
+        <v>0.538144982589427</v>
       </c>
       <c r="F10" t="n">
-        <v>33975</v>
+        <v>33035</v>
       </c>
       <c r="G10" t="n">
-        <v>36292</v>
+        <v>35352</v>
       </c>
       <c r="H10" t="n">
-        <v>51176</v>
+        <v>50236</v>
       </c>
       <c r="I10" t="n">
-        <v>74765</v>
+        <v>73825</v>
       </c>
       <c r="J10" t="n">
-        <v>87513</v>
+        <v>86573</v>
       </c>
       <c r="K10" t="n">
-        <v>97958</v>
+        <v>97018</v>
       </c>
       <c r="L10" t="n">
-        <v>91744</v>
+        <v>90804</v>
       </c>
       <c r="M10" t="n">
-        <v>68872</v>
+        <v>67932</v>
       </c>
       <c r="N10" t="n">
-        <v>62607</v>
+        <v>61667</v>
       </c>
       <c r="O10" t="n">
-        <v>65884</v>
+        <v>64944</v>
       </c>
       <c r="P10" t="n">
-        <v>57431</v>
+        <v>56491</v>
       </c>
       <c r="Q10" t="n">
-        <v>43124</v>
+        <v>42184</v>
       </c>
     </row>
     <row r="11">
@@ -983,49 +983,49 @@
         <v>649555</v>
       </c>
       <c r="C11" t="n">
-        <v>299984</v>
+        <v>357614</v>
       </c>
       <c r="D11" t="n">
-        <v>349571</v>
+        <v>291941</v>
       </c>
       <c r="E11" t="n">
-        <v>0.538169977907952</v>
+        <v>0.449447698809185</v>
       </c>
       <c r="F11" t="n">
-        <v>110329</v>
+        <v>105526</v>
       </c>
       <c r="G11" t="n">
-        <v>147134</v>
+        <v>142331</v>
       </c>
       <c r="H11" t="n">
-        <v>234152</v>
+        <v>229349</v>
       </c>
       <c r="I11" t="n">
-        <v>325013</v>
+        <v>320210</v>
       </c>
       <c r="J11" t="n">
-        <v>354114</v>
+        <v>349311</v>
       </c>
       <c r="K11" t="n">
-        <v>457027</v>
+        <v>452224</v>
       </c>
       <c r="L11" t="n">
-        <v>440347</v>
+        <v>435544</v>
       </c>
       <c r="M11" t="n">
-        <v>353585</v>
+        <v>348782</v>
       </c>
       <c r="N11" t="n">
-        <v>233937</v>
+        <v>229134</v>
       </c>
       <c r="O11" t="n">
-        <v>297312</v>
+        <v>292509</v>
       </c>
       <c r="P11" t="n">
-        <v>395119</v>
+        <v>390316</v>
       </c>
       <c r="Q11" t="n">
-        <v>328783</v>
+        <v>323980</v>
       </c>
     </row>
     <row r="12">
@@ -1036,49 +1036,49 @@
         <v>1536924</v>
       </c>
       <c r="C12" t="n">
-        <v>772974</v>
+        <v>870980</v>
       </c>
       <c r="D12" t="n">
-        <v>763950</v>
+        <v>665944</v>
       </c>
       <c r="E12" t="n">
-        <v>0.497064266027468</v>
+        <v>0.433296636658677</v>
       </c>
       <c r="F12" t="n">
-        <v>227221</v>
+        <v>219054</v>
       </c>
       <c r="G12" t="n">
-        <v>380541</v>
+        <v>372374</v>
       </c>
       <c r="H12" t="n">
-        <v>487348</v>
+        <v>479181</v>
       </c>
       <c r="I12" t="n">
-        <v>850661</v>
+        <v>842494</v>
       </c>
       <c r="J12" t="n">
-        <v>866180</v>
+        <v>858013</v>
       </c>
       <c r="K12" t="n">
-        <v>1112542</v>
+        <v>1104375</v>
       </c>
       <c r="L12" t="n">
-        <v>1072715</v>
+        <v>1064548</v>
       </c>
       <c r="M12" t="n">
-        <v>908816</v>
+        <v>900649</v>
       </c>
       <c r="N12" t="n">
-        <v>874507</v>
+        <v>866340</v>
       </c>
       <c r="O12" t="n">
-        <v>745867</v>
+        <v>737700</v>
       </c>
       <c r="P12" t="n">
-        <v>598593</v>
+        <v>590426</v>
       </c>
       <c r="Q12" t="n">
-        <v>514688</v>
+        <v>506521</v>
       </c>
     </row>
     <row r="13">
@@ -1089,49 +1089,49 @@
         <v>451340</v>
       </c>
       <c r="C13" t="n">
-        <v>166128</v>
+        <v>190656</v>
       </c>
       <c r="D13" t="n">
-        <v>285212</v>
+        <v>260684</v>
       </c>
       <c r="E13" t="n">
-        <v>0.63192271901449</v>
+        <v>0.577577879204148</v>
       </c>
       <c r="F13" t="n">
-        <v>121105</v>
+        <v>119061</v>
       </c>
       <c r="G13" t="n">
-        <v>98938</v>
+        <v>96894</v>
       </c>
       <c r="H13" t="n">
-        <v>121779</v>
+        <v>119735</v>
       </c>
       <c r="I13" t="n">
-        <v>171272</v>
+        <v>169228</v>
       </c>
       <c r="J13" t="n">
-        <v>142874</v>
+        <v>140830</v>
       </c>
       <c r="K13" t="n">
-        <v>185698</v>
+        <v>183654</v>
       </c>
       <c r="L13" t="n">
-        <v>187057</v>
+        <v>185013</v>
       </c>
       <c r="M13" t="n">
-        <v>191459</v>
+        <v>189415</v>
       </c>
       <c r="N13" t="n">
-        <v>167415</v>
+        <v>165371</v>
       </c>
       <c r="O13" t="n">
-        <v>203741</v>
+        <v>201697</v>
       </c>
       <c r="P13" t="n">
-        <v>217250</v>
+        <v>215206</v>
       </c>
       <c r="Q13" t="n">
-        <v>155842</v>
+        <v>153798</v>
       </c>
     </row>
     <row r="14">
@@ -1142,49 +1142,49 @@
         <v>95534</v>
       </c>
       <c r="C14" t="n">
-        <v>40954</v>
+        <v>49812</v>
       </c>
       <c r="D14" t="n">
-        <v>54580</v>
+        <v>45722</v>
       </c>
       <c r="E14" t="n">
-        <v>0.571314924529487</v>
+        <v>0.478594008415852</v>
       </c>
       <c r="F14" t="n">
-        <v>12894</v>
+        <v>12156</v>
       </c>
       <c r="G14" t="n">
-        <v>23288</v>
+        <v>22550</v>
       </c>
       <c r="H14" t="n">
-        <v>42288</v>
+        <v>41550</v>
       </c>
       <c r="I14" t="n">
-        <v>55166</v>
+        <v>54428</v>
       </c>
       <c r="J14" t="n">
-        <v>49649</v>
+        <v>48911</v>
       </c>
       <c r="K14" t="n">
-        <v>63205</v>
+        <v>62467</v>
       </c>
       <c r="L14" t="n">
-        <v>65521</v>
+        <v>64783</v>
       </c>
       <c r="M14" t="n">
-        <v>49546</v>
+        <v>48808</v>
       </c>
       <c r="N14" t="n">
-        <v>28246</v>
+        <v>27508</v>
       </c>
       <c r="O14" t="n">
-        <v>30338</v>
+        <v>29600</v>
       </c>
       <c r="P14" t="n">
-        <v>39098</v>
+        <v>38360</v>
       </c>
       <c r="Q14" t="n">
-        <v>33030</v>
+        <v>32292</v>
       </c>
     </row>
     <row r="15">
@@ -1195,49 +1195,49 @@
         <v>523435</v>
       </c>
       <c r="C15" t="n">
-        <v>113485</v>
+        <v>140214</v>
       </c>
       <c r="D15" t="n">
-        <v>409950</v>
+        <v>383221</v>
       </c>
       <c r="E15" t="n">
-        <v>0.783191800319046</v>
+        <v>0.732127198219454</v>
       </c>
       <c r="F15" t="n">
-        <v>138093</v>
+        <v>135866</v>
       </c>
       <c r="G15" t="n">
-        <v>120872</v>
+        <v>118645</v>
       </c>
       <c r="H15" t="n">
-        <v>130960</v>
+        <v>128733</v>
       </c>
       <c r="I15" t="n">
-        <v>179527</v>
+        <v>177300</v>
       </c>
       <c r="J15" t="n">
-        <v>162169</v>
+        <v>159942</v>
       </c>
       <c r="K15" t="n">
-        <v>157023</v>
+        <v>154796</v>
       </c>
       <c r="L15" t="n">
-        <v>192811</v>
+        <v>190584</v>
       </c>
       <c r="M15" t="n">
-        <v>171307</v>
+        <v>169080</v>
       </c>
       <c r="N15" t="n">
-        <v>152878</v>
+        <v>150651</v>
       </c>
       <c r="O15" t="n">
-        <v>135226</v>
+        <v>132999</v>
       </c>
       <c r="P15" t="n">
-        <v>163614</v>
+        <v>161387</v>
       </c>
       <c r="Q15" t="n">
-        <v>142334</v>
+        <v>140107</v>
       </c>
     </row>
     <row r="16">
@@ -1248,49 +1248,49 @@
         <v>201735</v>
       </c>
       <c r="C16" t="n">
-        <v>71769</v>
+        <v>85701</v>
       </c>
       <c r="D16" t="n">
-        <v>129966</v>
+        <v>116034</v>
       </c>
       <c r="E16" t="n">
-        <v>0.644241207524723</v>
+        <v>0.575180310803777</v>
       </c>
       <c r="F16" t="n">
-        <v>46957</v>
+        <v>45797</v>
       </c>
       <c r="G16" t="n">
-        <v>57531</v>
+        <v>56371</v>
       </c>
       <c r="H16" t="n">
-        <v>56186</v>
+        <v>55026</v>
       </c>
       <c r="I16" t="n">
-        <v>93282</v>
+        <v>92122</v>
       </c>
       <c r="J16" t="n">
-        <v>94770</v>
+        <v>93610</v>
       </c>
       <c r="K16" t="n">
-        <v>114224</v>
+        <v>113064</v>
       </c>
       <c r="L16" t="n">
-        <v>109475</v>
+        <v>108315</v>
       </c>
       <c r="M16" t="n">
-        <v>91657</v>
+        <v>90497</v>
       </c>
       <c r="N16" t="n">
-        <v>85526</v>
+        <v>84366</v>
       </c>
       <c r="O16" t="n">
-        <v>87677</v>
+        <v>86517</v>
       </c>
       <c r="P16" t="n">
-        <v>95700</v>
+        <v>94540</v>
       </c>
       <c r="Q16" t="n">
-        <v>83584</v>
+        <v>82424</v>
       </c>
     </row>
     <row r="17">
@@ -1301,49 +1301,49 @@
         <v>321165</v>
       </c>
       <c r="C17" t="n">
-        <v>157896</v>
+        <v>177262</v>
       </c>
       <c r="D17" t="n">
-        <v>163269</v>
+        <v>143903</v>
       </c>
       <c r="E17" t="n">
-        <v>0.508364859184531</v>
+        <v>0.448065636043778</v>
       </c>
       <c r="F17" t="n">
-        <v>77007</v>
+        <v>75393</v>
       </c>
       <c r="G17" t="n">
-        <v>87249</v>
+        <v>85635</v>
       </c>
       <c r="H17" t="n">
-        <v>67753</v>
+        <v>66139</v>
       </c>
       <c r="I17" t="n">
-        <v>138973</v>
+        <v>137359</v>
       </c>
       <c r="J17" t="n">
-        <v>110386</v>
+        <v>108772</v>
       </c>
       <c r="K17" t="n">
-        <v>134370</v>
+        <v>132756</v>
       </c>
       <c r="L17" t="n">
-        <v>145330</v>
+        <v>143716</v>
       </c>
       <c r="M17" t="n">
-        <v>130172</v>
+        <v>128558</v>
       </c>
       <c r="N17" t="n">
-        <v>131639</v>
+        <v>130025</v>
       </c>
       <c r="O17" t="n">
-        <v>143994</v>
+        <v>142380</v>
       </c>
       <c r="P17" t="n">
-        <v>138575</v>
+        <v>136961</v>
       </c>
       <c r="Q17" t="n">
-        <v>101897</v>
+        <v>100283</v>
       </c>
     </row>
     <row r="18">
@@ -1354,49 +1354,49 @@
         <v>289899</v>
       </c>
       <c r="C18" t="n">
-        <v>99160</v>
+        <v>122906</v>
       </c>
       <c r="D18" t="n">
-        <v>190739</v>
+        <v>166993</v>
       </c>
       <c r="E18" t="n">
-        <v>0.657949837702096</v>
+        <v>0.576038551357542</v>
       </c>
       <c r="F18" t="n">
-        <v>58471</v>
+        <v>56492</v>
       </c>
       <c r="G18" t="n">
-        <v>48500</v>
+        <v>46521</v>
       </c>
       <c r="H18" t="n">
-        <v>51624</v>
+        <v>49645</v>
       </c>
       <c r="I18" t="n">
-        <v>73866</v>
+        <v>71887</v>
       </c>
       <c r="J18" t="n">
-        <v>80195</v>
+        <v>78216</v>
       </c>
       <c r="K18" t="n">
-        <v>88957</v>
+        <v>86978</v>
       </c>
       <c r="L18" t="n">
-        <v>89891</v>
+        <v>87912</v>
       </c>
       <c r="M18" t="n">
-        <v>88584</v>
+        <v>86605</v>
       </c>
       <c r="N18" t="n">
-        <v>100564</v>
+        <v>98585</v>
       </c>
       <c r="O18" t="n">
-        <v>101025</v>
+        <v>99046</v>
       </c>
       <c r="P18" t="n">
-        <v>110477</v>
+        <v>108498</v>
       </c>
       <c r="Q18" t="n">
-        <v>86245</v>
+        <v>84266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>